<commit_message>
Added config, price selectors and price sorting
</commit_message>
<xml_diff>
--- a/RPA_RentOffersGenerator/results.xlsx
+++ b/RPA_RentOffersGenerator/results.xlsx
@@ -21,21 +21,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X95F000FI</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-XCG610086</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X9PL102S0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102TD</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102SK</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+  <x:si>
+    <x:t>Garsoniera str.Parang, et.3, mobilat, utilat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>180 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-XB7200028</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Inchiriere Apartament 1 camera semidecomandat, 25 mp, Etajul 4 din 4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>200 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X01V104V9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garsoniera, Manastur</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X9PL1035U</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apartament 1 camera str.Bucegi, zona McDonald;s, decomandat</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-XARU0004J</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Garsoniera in zona Piata Flora</x:t>
+  </x:si>
+  <x:si>
+    <x:t>230 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X8M2103DP</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -396,29 +420,59 @@
     <x:col min="1" max="1" width="187.363281" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <x:c r="A1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="2" t="s">
+        <x:v>2</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:1">
+    <x:row r="2" spans="1:3">
       <x:c r="A2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C2" s="2" t="s">
+        <x:v>5</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" x14ac:dyDescent="0.35">
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <x:c r="A3" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C3" s="2" t="s">
+        <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1">
+    <x:row r="4" spans="1:3">
       <x:c r="A4" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
+      <x:c r="C4" s="2" t="s">
+        <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" x14ac:dyDescent="0.35">
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <x:c r="A5" s="2" t="s">
-        <x:v>4</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="C5" s="2" t="s">
+        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Added selecting number of rooms
</commit_message>
<xml_diff>
--- a/RPA_RentOffersGenerator/results.xlsx
+++ b/RPA_RentOffersGenerator/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <x:workbook xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <x:fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <x:workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/644335611823a40d/Desktop/Facultate/Semestrul5/RPA/RPA_RentOffersGenerator/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/644335611823a40d/Desktop/Facultate/Semestrul5/RPA/RPA_PROJECT_RentOffersGenerator/RPA_RentOffersGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_E0FA62E8C631FD4A046BE230A1E4A85B4BE42A31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C26A81A7-8F9C-4A0D-98D9-FF3EFF4AC636}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_E0FA62E8C631FD4A046BE230A1E4A85B4BE42A31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{053C3DB9-9643-46A5-86AF-FD5B4D9AD98C}"/>
   <x:bookViews>
-    <x:workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <x:workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
   <x:sheets>
     <x:sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -21,45 +21,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
-    <x:t>Garsoniera str.Parang, et.3, mobilat, utilat</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X9PL10363</x:t>
   </x:si>
   <x:si>
-    <x:t>180 EUR / lună</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F91030E</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-XB7200028</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102TD</x:t>
   </x:si>
   <x:si>
-    <x:t>Inchiriere Apartament 1 camera semidecomandat, 25 mp, Etajul 4 din 4</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102SK</x:t>
   </x:si>
   <x:si>
-    <x:t>200 EUR / lună</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X01V104V9</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Garsoniera, Manastur</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X9PL1035U</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Apartament 1 camera str.Bucegi, zona McDonald;s, decomandat</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-XARU0004J</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Garsoniera in zona Piata Flora</x:t>
-  </x:si>
-  <x:si>
-    <x:t>230 EUR / lună</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-garsoniere/cluj-napoca/manastur/garsoniera-de-inchiriat-X8M2103DP</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102VU</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -411,68 +387,42 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:A5"/>
+  <x:dimension ref="A1:C5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0"/>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A1" sqref="A1 A1:A1 A1:C5"/>
+    </x:sheetView>
   </x:sheetViews>
-  <x:sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
-    <x:col min="1" max="1" width="187.363281" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="1" max="1" width="58.425781" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="13.710938" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="99" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <x:c r="A1" s="2" t="s">
+    <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C1" s="2" t="s">
         <x:v>0</x:v>
       </x:c>
-      <x:c r="B1" s="2" t="s">
+    </x:row>
+    <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
-      <x:c r="C1" s="2" t="s">
+    </x:row>
+    <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C3" s="2" t="s">
         <x:v>2</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:3">
-      <x:c r="A2" s="2" t="s">
+    <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C4" s="2" t="s">
         <x:v>3</x:v>
       </x:c>
-      <x:c r="B2" s="2" t="s">
+    </x:row>
+    <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="C5" s="2" t="s">
         <x:v>4</x:v>
-      </x:c>
-      <x:c r="C2" s="2" t="s">
-        <x:v>5</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <x:c r="A3" s="2" t="s">
-        <x:v>6</x:v>
-      </x:c>
-      <x:c r="B3" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C3" s="2" t="s">
-        <x:v>7</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:3">
-      <x:c r="A4" s="2" t="s">
-        <x:v>8</x:v>
-      </x:c>
-      <x:c r="B4" s="2" t="s">
-        <x:v>4</x:v>
-      </x:c>
-      <x:c r="C4" s="2" t="s">
-        <x:v>9</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <x:c r="A5" s="2" t="s">
-        <x:v>10</x:v>
-      </x:c>
-      <x:c r="B5" s="2" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C5" s="2" t="s">
-        <x:v>12</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Broke Main workflow into more workflows - renamed activities
</commit_message>
<xml_diff>
--- a/RPA_RentOffersGenerator/results.xlsx
+++ b/RPA_RentOffersGenerator/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/644335611823a40d/Desktop/Facultate/Semestrul5/RPA/RPA_PROJECT_RentOffersGenerator/RPA_RentOffersGenerator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_E0FA62E8C631FD4A046BE230A1E4A85B4BE42A31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{053C3DB9-9643-46A5-86AF-FD5B4D9AD98C}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_E0FA62E8C631FD4A046BE230A1E4A85B4BE42A31" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1DB4EA65-25CF-48DB-BE4D-A72FE00A9B6C}"/>
   <x:bookViews>
     <x:workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" firstSheet="0" activeTab="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </x:bookViews>
@@ -23,19 +23,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X9PL10363</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/buna-ziua/apartament-de-inchiriat-2-camere-XBB800047</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F91030E</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-X8FG10042</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102TD</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-XBNT102IT</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102SK</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/europa/apartament-de-inchiriat-2-camere-X8FG1005O</x:t>
   </x:si>
   <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X7F9102VU</x:t>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-X8FG1005P</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -389,15 +389,15 @@
   </x:sheetPr>
   <x:dimension ref="A1:C5"/>
   <x:sheetViews>
-    <x:sheetView tabSelected="1" workbookViewId="0">
-      <x:selection activeCell="A1" sqref="A1 A1:A1 A1:C5"/>
+    <x:sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <x:selection activeCell="A11" sqref="A11 A11:A11"/>
     </x:sheetView>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:cols>
     <x:col min="1" max="1" width="58.425781" style="2" bestFit="1" customWidth="1"/>
     <x:col min="2" max="2" width="13.710938" style="2" bestFit="1" customWidth="1"/>
-    <x:col min="3" max="3" width="99" style="2" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="110.855469" style="2" bestFit="1" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -425,6 +425,7 @@
         <x:v>4</x:v>
       </x:c>
     </x:row>
+    <x:row r="11" spans="1:3"/>
   </x:sheetData>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="0.75" bottom="0.5" header="0.5" footer="0.75"/>

</xml_diff>

<commit_message>
Somehow made it work
</commit_message>
<xml_diff>
--- a/RPA_RentOffersGenerator/results.xlsx
+++ b/RPA_RentOffersGenerator/results.xlsx
@@ -21,21 +21,48 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/buna-ziua/apartament-de-inchiriat-2-camere-XBB800047</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-X8FG10042</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-XBNT102IT</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/europa/apartament-de-inchiriat-2-camere-X8FG1005O</x:t>
-  </x:si>
-  <x:si>
-    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/gheorgheni/apartament-de-inchiriat-2-camere-X8FG1005P</x:t>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <x:si>
+    <x:t>Garsoniera, 32mp, cartier Manastur, zon Big</x:t>
+  </x:si>
+  <x:si>
+    <x:t>230 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X5NQ1022U</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apartament 2 camere, recent renovat, 37mp, Manastur , Pet friendly</x:t>
+  </x:si>
+  <x:si>
+    <x:t>240 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X3SH10DA2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apartament 2 camere , modest , mobilat-utilat!!!</x:t>
+  </x:si>
+  <x:si>
+    <x:t>250 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-XAON100FG</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apartament 2 camere, decomandat, 45 mp, pet friendly, zona strazii...</x:t>
+  </x:si>
+  <x:si>
+    <x:t>270 EUR / lună</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-X3SH10DDL</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Apartament 2 camere Manastur, str. Tasnad, zona Cora, partial mobilat, cu GARAJ</x:t>
+  </x:si>
+  <x:si>
+    <x:t>https://www.imobiliare.ro/inchirieri-apartamente/cluj-napoca/manastur/apartament-de-inchiriat-2-camere-XARU0003Q</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -401,28 +428,58 @@
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="2" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="2" t="s">
+        <x:v>1</x:v>
+      </x:c>
       <x:c r="C1" s="2" t="s">
-        <x:v>0</x:v>
+        <x:v>2</x:v>
       </x:c>
     </x:row>
     <x:row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="2" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="B2" s="2" t="s">
+        <x:v>4</x:v>
+      </x:c>
       <x:c r="C2" s="2" t="s">
-        <x:v>1</x:v>
+        <x:v>5</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="2" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="B3" s="2" t="s">
+        <x:v>7</x:v>
+      </x:c>
       <x:c r="C3" s="2" t="s">
-        <x:v>2</x:v>
+        <x:v>8</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="2" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
       <x:c r="C4" s="2" t="s">
-        <x:v>3</x:v>
+        <x:v>11</x:v>
       </x:c>
     </x:row>
     <x:row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <x:c r="A5" s="2" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B5" s="2" t="s">
+        <x:v>10</x:v>
+      </x:c>
       <x:c r="C5" s="2" t="s">
-        <x:v>4</x:v>
+        <x:v>13</x:v>
       </x:c>
     </x:row>
     <x:row r="11" spans="1:3"/>

</xml_diff>